<commit_message>
Estadisticos Segundo Parcial Sin Ameca
</commit_message>
<xml_diff>
--- a/academias/Inglés - Estadisticos 20242.xlsx
+++ b/academias/Inglés - Estadisticos 20242.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="44">
   <si>
     <t>Docente</t>
   </si>
@@ -51,21 +51,27 @@
     <t>por_blancos</t>
   </si>
   <si>
-    <t>Ameca Garcia Ivan</t>
-  </si>
-  <si>
     <t>Avila Coronado Julieta</t>
   </si>
   <si>
+    <t>Domínguez Burgos Marioscar</t>
+  </si>
+  <si>
     <t>González Nuñez Veronica</t>
   </si>
   <si>
+    <t>Pesce Bautista Victor Manuel</t>
+  </si>
+  <si>
     <t>Rosas Aguilar Claudia Leonor</t>
   </si>
   <si>
     <t>Ruiz Delgado Nemi</t>
   </si>
   <si>
+    <t>Zarate Amezcua Eladio Jorge</t>
+  </si>
+  <si>
     <t>Ingles II</t>
   </si>
   <si>
@@ -81,67 +87,67 @@
     <t>2AEV</t>
   </si>
   <si>
+    <t>4AEM</t>
+  </si>
+  <si>
+    <t>4ALCM</t>
+  </si>
+  <si>
+    <t>4APM</t>
+  </si>
+  <si>
+    <t>4BEM</t>
+  </si>
+  <si>
     <t>2ALCV</t>
   </si>
   <si>
     <t>2APV</t>
   </si>
   <si>
+    <t>4AEV</t>
+  </si>
+  <si>
+    <t>4ALCV</t>
+  </si>
+  <si>
+    <t>4APV</t>
+  </si>
+  <si>
+    <t>4ARHV</t>
+  </si>
+  <si>
+    <t>4ASV</t>
+  </si>
+  <si>
+    <t>2ASV</t>
+  </si>
+  <si>
+    <t>2AEM</t>
+  </si>
+  <si>
+    <t>2ALCM</t>
+  </si>
+  <si>
+    <t>2APM</t>
+  </si>
+  <si>
+    <t>2BEM</t>
+  </si>
+  <si>
+    <t>2ARHM</t>
+  </si>
+  <si>
+    <t>2BLCM</t>
+  </si>
+  <si>
+    <t>4ARHM</t>
+  </si>
+  <si>
+    <t>4BLCM</t>
+  </si>
+  <si>
     <t>2ARHV</t>
-  </si>
-  <si>
-    <t>2ASV</t>
-  </si>
-  <si>
-    <t>4AEV</t>
-  </si>
-  <si>
-    <t>4AEM</t>
-  </si>
-  <si>
-    <t>4ALCM</t>
-  </si>
-  <si>
-    <t>4APM</t>
-  </si>
-  <si>
-    <t>4BEM</t>
-  </si>
-  <si>
-    <t>4ALCV</t>
-  </si>
-  <si>
-    <t>4APV</t>
-  </si>
-  <si>
-    <t>4ARHV</t>
-  </si>
-  <si>
-    <t>4ASV</t>
-  </si>
-  <si>
-    <t>2AEM</t>
-  </si>
-  <si>
-    <t>2ALCM</t>
-  </si>
-  <si>
-    <t>2APM</t>
-  </si>
-  <si>
-    <t>2BEM</t>
-  </si>
-  <si>
-    <t>2ARHM</t>
-  </si>
-  <si>
-    <t>2BLCM</t>
-  </si>
-  <si>
-    <t>4ARHM</t>
-  </si>
-  <si>
-    <t>4BLCM</t>
   </si>
 </sst>
 </file>
@@ -505,7 +511,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -558,10 +564,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>36</v>
@@ -593,28 +599,28 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D3">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E3">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F3">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
-        <v>42.9</v>
+        <v>95.8</v>
       </c>
       <c r="H3" s="1">
-        <v>57.1</v>
+        <v>4.2</v>
       </c>
       <c r="I3" s="2">
-        <v>5.7</v>
+        <v>8.4</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -628,28 +634,28 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E4">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1">
-        <v>69.59999999999999</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="H4" s="1">
-        <v>30.4</v>
+        <v>5.9</v>
       </c>
       <c r="I4" s="2">
-        <v>6.5</v>
+        <v>8.4</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -663,28 +669,28 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F5">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1">
-        <v>56.7</v>
+        <v>93.5</v>
       </c>
       <c r="H5" s="1">
-        <v>43.3</v>
+        <v>6.5</v>
       </c>
       <c r="I5" s="2">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -698,28 +704,28 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
         <v>24</v>
       </c>
-      <c r="D6">
-        <v>11</v>
-      </c>
       <c r="E6">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>90.90000000000001</v>
+        <v>95.8</v>
       </c>
       <c r="H6" s="1">
-        <v>9.1</v>
+        <v>4.2</v>
       </c>
       <c r="I6" s="2">
-        <v>6.5</v>
+        <v>8.6</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -733,28 +739,25 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D7">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="E7">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="F7">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1">
-        <v>36.8</v>
+        <v>84.59999999999999</v>
       </c>
       <c r="H7" s="1">
-        <v>63.2</v>
+        <v>15.4</v>
       </c>
       <c r="I7" s="2">
-        <v>5.5</v>
+        <v>7.7</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -765,28 +768,31 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
       <c r="D8">
-        <v>147</v>
+        <v>28</v>
       </c>
       <c r="E8">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="F8">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="G8" s="1">
-        <v>55.1</v>
+        <v>42.9</v>
       </c>
       <c r="H8" s="1">
-        <v>44.9</v>
+        <v>57.1</v>
       </c>
       <c r="I8" s="2">
-        <v>6.1</v>
+        <v>5.7</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -800,28 +806,25 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E9">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G9" s="1">
-        <v>95.8</v>
+        <v>42.9</v>
       </c>
       <c r="H9" s="1">
-        <v>4.2</v>
+        <v>57.1</v>
       </c>
       <c r="I9" s="2">
-        <v>8.4</v>
+        <v>5.7</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -832,31 +835,31 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E10">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G10" s="1">
-        <v>94.09999999999999</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="H10" s="1">
-        <v>5.9</v>
+        <v>30.4</v>
       </c>
       <c r="I10" s="2">
-        <v>8.4</v>
+        <v>6.5</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -867,31 +870,31 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11">
-        <v>31</v>
-      </c>
-      <c r="E11">
-        <v>29</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
       <c r="G11" s="1">
-        <v>93.5</v>
+        <v>36.8</v>
       </c>
       <c r="H11" s="1">
-        <v>6.5</v>
+        <v>63.2</v>
       </c>
       <c r="I11" s="2">
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -902,31 +905,31 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>13</v>
+      </c>
+      <c r="F12">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12">
-        <v>24</v>
-      </c>
-      <c r="E12">
-        <v>23</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
       <c r="G12" s="1">
-        <v>95.8</v>
+        <v>52</v>
       </c>
       <c r="H12" s="1">
-        <v>4.2</v>
+        <v>48</v>
       </c>
       <c r="I12" s="2">
-        <v>8.6</v>
+        <v>6.3</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -937,28 +940,31 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
       </c>
       <c r="D13">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="E13">
-        <v>107</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G13" s="1">
-        <v>94.7</v>
+        <v>61.5</v>
       </c>
       <c r="H13" s="1">
-        <v>5.3</v>
+        <v>38.5</v>
       </c>
       <c r="I13" s="2">
-        <v>8.199999999999999</v>
+        <v>6.2</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -972,28 +978,28 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D14">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F14">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="H14" s="1">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="I14" s="2">
-        <v>6.3</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1007,28 +1013,28 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D15">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E15">
         <v>8</v>
       </c>
       <c r="F15">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G15" s="1">
-        <v>61.5</v>
+        <v>80</v>
       </c>
       <c r="H15" s="1">
-        <v>38.5</v>
+        <v>20</v>
       </c>
       <c r="I15" s="2">
-        <v>6.2</v>
+        <v>6.8</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1042,28 +1048,25 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D16">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="E16">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="G16" s="1">
-        <v>100</v>
+        <v>63.5</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>36.5</v>
       </c>
       <c r="I16" s="2">
-        <v>9.300000000000001</v>
+        <v>6.8</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1074,31 +1077,31 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17">
+        <v>11</v>
+      </c>
+      <c r="E17">
         <v>10</v>
       </c>
-      <c r="E17">
-        <v>8</v>
-      </c>
       <c r="F17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" s="1">
-        <v>80</v>
+        <v>90.90000000000001</v>
       </c>
       <c r="H17" s="1">
-        <v>20</v>
+        <v>9.1</v>
       </c>
       <c r="I17" s="2">
-        <v>6.8</v>
+        <v>6.5</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -1109,28 +1112,28 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D18">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="E18">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="F18">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G18" s="1">
-        <v>69.40000000000001</v>
+        <v>90.90000000000001</v>
       </c>
       <c r="H18" s="1">
-        <v>30.6</v>
+        <v>9.1</v>
       </c>
       <c r="I18" s="2">
-        <v>7.2</v>
+        <v>6.5</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -1141,13 +1144,13 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19">
         <v>37</v>
@@ -1176,13 +1179,13 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D20">
         <v>39</v>
@@ -1211,13 +1214,13 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D21">
         <v>32</v>
@@ -1246,13 +1249,13 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D22">
         <v>39</v>
@@ -1281,10 +1284,10 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D23">
         <v>147</v>
@@ -1313,13 +1316,13 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D24">
         <v>49</v>
@@ -1348,13 +1351,13 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D25">
         <v>38</v>
@@ -1383,13 +1386,13 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D26">
         <v>40</v>
@@ -1418,13 +1421,13 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D27">
         <v>38</v>
@@ -1453,10 +1456,10 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D28">
         <v>165</v>
@@ -1484,31 +1487,98 @@
       </c>
     </row>
     <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
       </c>
       <c r="D29">
+        <v>30</v>
+      </c>
+      <c r="E29">
+        <v>17</v>
+      </c>
+      <c r="F29">
+        <v>13</v>
+      </c>
+      <c r="G29" s="1">
+        <v>56.7</v>
+      </c>
+      <c r="H29" s="1">
+        <v>43.3</v>
+      </c>
+      <c r="I29" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30">
+        <v>30</v>
+      </c>
+      <c r="E30">
+        <v>17</v>
+      </c>
+      <c r="F30">
+        <v>13</v>
+      </c>
+      <c r="G30" s="1">
+        <v>56.7</v>
+      </c>
+      <c r="H30" s="1">
+        <v>43.3</v>
+      </c>
+      <c r="I30" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31">
         <v>634</v>
       </c>
-      <c r="E29">
+      <c r="E31">
         <v>508</v>
       </c>
-      <c r="F29">
+      <c r="F31">
         <v>126</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G31" s="1">
         <v>80.09999999999999</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H31" s="1">
         <v>19.9</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I31" s="2">
         <v>7.3</v>
       </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29" s="1">
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1519,7 +1589,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1571,10 +1641,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>36</v>
@@ -1606,28 +1676,28 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>24</v>
+      </c>
+      <c r="E3">
         <v>21</v>
       </c>
-      <c r="D3">
-        <v>28</v>
-      </c>
-      <c r="E3">
-        <v>22</v>
-      </c>
       <c r="F3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G3" s="1">
-        <v>78.59999999999999</v>
+        <v>87.5</v>
       </c>
       <c r="H3" s="1">
-        <v>21.4</v>
+        <v>12.5</v>
       </c>
       <c r="I3" s="2">
-        <v>7.5</v>
+        <v>7.4</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1641,28 +1711,28 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E4">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1">
-        <v>78.3</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="H4" s="1">
-        <v>21.7</v>
+        <v>5.9</v>
       </c>
       <c r="I4" s="2">
-        <v>7.1</v>
+        <v>9.1</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1676,25 +1746,25 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1">
-        <v>100</v>
+        <v>93.5</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="I5" s="2">
         <v>8</v>
@@ -1711,16 +1781,16 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
         <v>24</v>
       </c>
-      <c r="D6">
-        <v>11</v>
-      </c>
       <c r="E6">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1732,7 +1802,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="2">
-        <v>7.1</v>
+        <v>8</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1746,28 +1816,25 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>149</v>
+      </c>
+      <c r="E7">
+        <v>132</v>
+      </c>
+      <c r="F7">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7">
-        <v>19</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>9</v>
-      </c>
       <c r="G7" s="1">
-        <v>52.6</v>
+        <v>88.59999999999999</v>
       </c>
       <c r="H7" s="1">
-        <v>47.4</v>
+        <v>11.4</v>
       </c>
       <c r="I7" s="2">
-        <v>6.7</v>
+        <v>8.1</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1778,28 +1845,31 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
       <c r="D8">
-        <v>147</v>
+        <v>28</v>
       </c>
       <c r="E8">
-        <v>117</v>
+        <v>22</v>
       </c>
       <c r="F8">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1">
-        <v>79.59999999999999</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="H8" s="1">
-        <v>20.4</v>
+        <v>21.4</v>
       </c>
       <c r="I8" s="2">
-        <v>7.4</v>
+        <v>7.5</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1813,28 +1883,25 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E9">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G9" s="1">
-        <v>87.5</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="H9" s="1">
-        <v>12.5</v>
+        <v>21.4</v>
       </c>
       <c r="I9" s="2">
-        <v>7.4</v>
+        <v>7.5</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1845,31 +1912,31 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E10">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G10" s="1">
-        <v>94.09999999999999</v>
+        <v>78.3</v>
       </c>
       <c r="H10" s="1">
-        <v>5.9</v>
+        <v>21.7</v>
       </c>
       <c r="I10" s="2">
-        <v>9.1</v>
+        <v>7.1</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1880,31 +1947,31 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E11">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G11" s="1">
-        <v>93.5</v>
+        <v>52.6</v>
       </c>
       <c r="H11" s="1">
-        <v>6.5</v>
+        <v>47.4</v>
       </c>
       <c r="I11" s="2">
-        <v>8</v>
+        <v>6.7</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1915,31 +1982,31 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E12">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G12" s="1">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="H12" s="1">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="I12" s="2">
-        <v>8</v>
+        <v>7.8</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1950,28 +2017,31 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
       </c>
       <c r="D13">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="E13">
-        <v>106</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G13" s="1">
-        <v>93.8</v>
+        <v>61.5</v>
       </c>
       <c r="H13" s="1">
-        <v>6.2</v>
+        <v>38.5</v>
       </c>
       <c r="I13" s="2">
-        <v>8.1</v>
+        <v>7.1</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1985,28 +2055,28 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D14">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E14">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F14">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="H14" s="1">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="I14" s="2">
-        <v>7.8</v>
+        <v>8.9</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -2020,28 +2090,28 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D15">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1">
-        <v>61.5</v>
+        <v>90</v>
       </c>
       <c r="H15" s="1">
-        <v>38.5</v>
+        <v>10</v>
       </c>
       <c r="I15" s="2">
-        <v>7.1</v>
+        <v>8.5</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -2055,28 +2125,25 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D16">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="E16">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G16" s="1">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="I16" s="2">
-        <v>8.9</v>
+        <v>7.7</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -2087,31 +2154,31 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E17">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="H17" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I17" s="2">
-        <v>8.5</v>
+        <v>7.1</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -2122,28 +2189,28 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D18">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="E18">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="F18">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="H18" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="I18" s="2">
-        <v>8.1</v>
+        <v>7.1</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -2154,13 +2221,13 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19">
         <v>37</v>
@@ -2189,13 +2256,13 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D20">
         <v>39</v>
@@ -2224,13 +2291,13 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D21">
         <v>32</v>
@@ -2259,13 +2326,13 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D22">
         <v>39</v>
@@ -2294,10 +2361,10 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D23">
         <v>147</v>
@@ -2326,13 +2393,13 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D24">
         <v>49</v>
@@ -2361,13 +2428,13 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D25">
         <v>38</v>
@@ -2396,13 +2463,13 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D26">
         <v>40</v>
@@ -2431,13 +2498,13 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D27">
         <v>38</v>
@@ -2466,10 +2533,10 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D28">
         <v>165</v>
@@ -2497,23 +2564,29 @@
       </c>
     </row>
     <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
       </c>
       <c r="D29">
-        <v>634</v>
+        <v>30</v>
       </c>
       <c r="E29">
-        <v>554</v>
+        <v>30</v>
       </c>
       <c r="F29">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G29" s="1">
-        <v>87.40000000000001</v>
+        <v>100</v>
       </c>
       <c r="H29" s="1">
-        <v>12.6</v>
+        <v>0</v>
       </c>
       <c r="I29" s="2">
         <v>8</v>
@@ -2522,6 +2595,67 @@
         <v>0</v>
       </c>
       <c r="K29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30">
+        <v>30</v>
+      </c>
+      <c r="E30">
+        <v>30</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>100</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2">
+        <v>8</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31">
+        <v>634</v>
+      </c>
+      <c r="E31">
+        <v>554</v>
+      </c>
+      <c r="F31">
+        <v>80</v>
+      </c>
+      <c r="G31" s="1">
+        <v>87.40000000000001</v>
+      </c>
+      <c r="H31" s="1">
+        <v>12.6</v>
+      </c>
+      <c r="I31" s="2">
+        <v>8</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2532,7 +2666,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2584,10 +2718,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>36</v>
@@ -2619,28 +2753,28 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>24</v>
+      </c>
+      <c r="E3">
         <v>21</v>
       </c>
-      <c r="D3">
-        <v>28</v>
-      </c>
-      <c r="E3">
-        <v>22</v>
-      </c>
       <c r="F3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G3" s="1">
-        <v>78.59999999999999</v>
+        <v>87.5</v>
       </c>
       <c r="H3" s="1">
-        <v>21.4</v>
+        <v>12.5</v>
       </c>
       <c r="I3" s="2">
-        <v>6.8</v>
+        <v>8</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -2654,28 +2788,28 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E4">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1">
-        <v>78.3</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="H4" s="1">
-        <v>21.7</v>
+        <v>5.9</v>
       </c>
       <c r="I4" s="2">
-        <v>7</v>
+        <v>8.9</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -2689,28 +2823,28 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1">
-        <v>100</v>
+        <v>93.5</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="I5" s="2">
-        <v>7.5</v>
+        <v>7.9</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -2724,16 +2858,16 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
         <v>24</v>
       </c>
-      <c r="D6">
-        <v>11</v>
-      </c>
       <c r="E6">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2745,7 +2879,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="2">
-        <v>7.2</v>
+        <v>8.5</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -2759,28 +2893,25 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>149</v>
+      </c>
+      <c r="E7">
+        <v>132</v>
+      </c>
+      <c r="F7">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7">
-        <v>19</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>9</v>
-      </c>
       <c r="G7" s="1">
-        <v>52.6</v>
+        <v>88.59999999999999</v>
       </c>
       <c r="H7" s="1">
-        <v>47.4</v>
+        <v>11.4</v>
       </c>
       <c r="I7" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -2791,28 +2922,31 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
       <c r="D8">
-        <v>147</v>
+        <v>28</v>
       </c>
       <c r="E8">
-        <v>117</v>
+        <v>22</v>
       </c>
       <c r="F8">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1">
-        <v>79.59999999999999</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="H8" s="1">
-        <v>20.4</v>
+        <v>21.4</v>
       </c>
       <c r="I8" s="2">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -2826,28 +2960,25 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E9">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G9" s="1">
-        <v>87.5</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="H9" s="1">
-        <v>12.5</v>
+        <v>21.4</v>
       </c>
       <c r="I9" s="2">
-        <v>8</v>
+        <v>6.8</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -2858,31 +2989,31 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E10">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G10" s="1">
-        <v>94.09999999999999</v>
+        <v>78.3</v>
       </c>
       <c r="H10" s="1">
-        <v>5.9</v>
+        <v>21.7</v>
       </c>
       <c r="I10" s="2">
-        <v>8.9</v>
+        <v>7</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -2893,31 +3024,31 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E11">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G11" s="1">
-        <v>93.5</v>
+        <v>52.6</v>
       </c>
       <c r="H11" s="1">
-        <v>6.5</v>
+        <v>47.4</v>
       </c>
       <c r="I11" s="2">
-        <v>7.9</v>
+        <v>6</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -2928,31 +3059,31 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E12">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G12" s="1">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="H12" s="1">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="I12" s="2">
-        <v>8.5</v>
+        <v>7.1</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -2963,28 +3094,31 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
       </c>
       <c r="D13">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="E13">
-        <v>106</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G13" s="1">
-        <v>93.8</v>
+        <v>61.5</v>
       </c>
       <c r="H13" s="1">
-        <v>6.2</v>
+        <v>38.5</v>
       </c>
       <c r="I13" s="2">
-        <v>8.300000000000001</v>
+        <v>6.6</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -2998,28 +3132,28 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D14">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E14">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F14">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="H14" s="1">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="I14" s="2">
-        <v>7.1</v>
+        <v>9.1</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -3033,28 +3167,28 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D15">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1">
-        <v>61.5</v>
+        <v>90</v>
       </c>
       <c r="H15" s="1">
-        <v>38.5</v>
+        <v>10</v>
       </c>
       <c r="I15" s="2">
-        <v>6.6</v>
+        <v>7.9</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -3068,28 +3202,25 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D16">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="E16">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G16" s="1">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="I16" s="2">
-        <v>9.1</v>
+        <v>7.3</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -3100,31 +3231,31 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E17">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="H17" s="1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I17" s="2">
-        <v>7.9</v>
+        <v>7.2</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -3135,28 +3266,28 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D18">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="E18">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="F18">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="H18" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="I18" s="2">
-        <v>7.7</v>
+        <v>7.2</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -3167,13 +3298,13 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19">
         <v>37</v>
@@ -3202,13 +3333,13 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D20">
         <v>39</v>
@@ -3237,13 +3368,13 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D21">
         <v>32</v>
@@ -3272,13 +3403,13 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D22">
         <v>39</v>
@@ -3307,10 +3438,10 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D23">
         <v>147</v>
@@ -3339,13 +3470,13 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D24">
         <v>49</v>
@@ -3374,13 +3505,13 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D25">
         <v>38</v>
@@ -3409,13 +3540,13 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D26">
         <v>40</v>
@@ -3444,13 +3575,13 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D27">
         <v>38</v>
@@ -3479,10 +3610,10 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D28">
         <v>165</v>
@@ -3510,31 +3641,98 @@
       </c>
     </row>
     <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
       </c>
       <c r="D29">
+        <v>30</v>
+      </c>
+      <c r="E29">
+        <v>30</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>100</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30">
+        <v>30</v>
+      </c>
+      <c r="E30">
+        <v>30</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>100</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31">
         <v>634</v>
       </c>
-      <c r="E29">
+      <c r="E31">
         <v>554</v>
       </c>
-      <c r="F29">
+      <c r="F31">
         <v>80</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G31" s="1">
         <v>87.40000000000001</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H31" s="1">
         <v>12.6</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I31" s="2">
         <v>7.8</v>
       </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29" s="1">
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>